<commit_message>
Add more cliches to list
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U037679\Documents\AnacondaProjects\conference_call_bingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\conference_call_bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6555" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6555" windowHeight="7800" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,13 @@
     <sheet name="fri" sheetId="7" state="hidden" r:id="rId7"/>
     <sheet name="mon1" sheetId="8" state="hidden" r:id="rId8"/>
     <sheet name="grid" sheetId="9" r:id="rId9"/>
-    <sheet name="grid1" sheetId="10" r:id="rId10"/>
-    <sheet name="grid2" sheetId="11" r:id="rId11"/>
-    <sheet name="grid3" sheetId="12" r:id="rId12"/>
-    <sheet name="grid4" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
   <si>
     <t>headers</t>
   </si>
@@ -172,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,11 +196,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -252,26 +243,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,9 +259,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -704,533 +677,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -1588,7 +1039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added one more to the list
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
   <si>
     <t xml:space="preserve">headers</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t xml:space="preserve">Keep _____ in the loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">awkward silence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“circle back”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“touch base”</t>
   </si>
   <si>
     <t xml:space="preserve">col0</t>
@@ -487,10 +496,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -697,6 +706,21 @@
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +882,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -927,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>19</v>
@@ -1002,7 +1026,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1071,7 +1095,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Rewrite by replacing openpyxl with xlsxwriter due to better formatting capabitlities
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
   <si>
     <t>headers</t>
   </si>
@@ -733,7 +733,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Tuesday</v>
+        <v>Happy Thursday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -1121,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,6 +1331,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create .py version for scheduling. Add flower box at top. Add win32 import at top.
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -9,23 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
-    <sheet name="paste here" sheetId="2" r:id="rId2"/>
-    <sheet name="list" sheetId="3" r:id="rId3"/>
-    <sheet name="mon" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="tue" sheetId="5" state="hidden" r:id="rId5"/>
-    <sheet name="wed" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="thu" sheetId="7" state="hidden" r:id="rId7"/>
-    <sheet name="fri" sheetId="8" state="hidden" r:id="rId8"/>
-    <sheet name="mon1" sheetId="9" state="hidden" r:id="rId9"/>
-    <sheet name="grid" sheetId="10" r:id="rId10"/>
+    <sheet name="list" sheetId="3" r:id="rId2"/>
+    <sheet name="mon" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="tue" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="wed" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="thu" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="fri" sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="mon1" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="grid" sheetId="10" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'paste here'!$B$2:$F$6</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
   <si>
     <t>headers</t>
   </si>
@@ -143,21 +139,12 @@
     <t>Ok. Let's get started</t>
   </si>
   <si>
-    <t>Happy [week]day!</t>
-  </si>
-  <si>
     <t>Can you reach out to  ____?</t>
   </si>
   <si>
-    <t>hit the ground running</t>
-  </si>
-  <si>
     <t>Loop in  _____</t>
   </si>
   <si>
-    <t>(At the beginning) This won't take the whole time</t>
-  </si>
-  <si>
     <t>Is _____ on the call?</t>
   </si>
   <si>
@@ -170,24 +157,12 @@
     <t>low hanging fruit</t>
   </si>
   <si>
-    <t>“circle back”</t>
-  </si>
-  <si>
     <t>I’ve got to jump on another call</t>
   </si>
   <si>
-    <t>“in flight”</t>
-  </si>
-  <si>
     <t>at the end of the day</t>
   </si>
   <si>
-    <t>“touch base”</t>
-  </si>
-  <si>
-    <t>“win-win”</t>
-  </si>
-  <si>
     <t>Sorry I’m late (lame excuse)</t>
   </si>
   <si>
@@ -252,9 +227,6 @@
   </si>
   <si>
     <t>level-set</t>
-  </si>
-  <si>
-    <t>This is the "final" format. Use this for the openpyxl styles.</t>
   </si>
   <si>
     <t>I have a hard stop</t>
@@ -733,7 +705,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Thursday</v>
+        <v>Happy Friday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -834,296 +806,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF70AD47"/>
-  </sheetPr>
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1135,12 +822,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1165,7 +852,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1175,7 +862,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -1195,7 +882,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -1205,22 +892,22 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1230,7 +917,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -1245,12 +932,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -1260,85 +947,101 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1410,22 +1113,6 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1437,7 +1124,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1489,7 +1176,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1506,7 +1193,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1523,7 +1210,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1540,7 +1227,143 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Add another cliche to the list.
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\conference_call_bingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\conference-call-bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>headers</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve">I'll give you back n minutes </t>
+  </si>
+  <si>
+    <t>[on a / It's been a] jouney</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Friday</v>
+        <v>Happy Tuesday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -808,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,6 +1026,11 @@
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and tweaked a few phrases; fixed Nick's email address
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\conference-call-bingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u037679\Documents\AnacondaProjects\conference-call-bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
   <si>
     <t>headers</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Ok. Let's get started</t>
   </si>
   <si>
-    <t>Can you reach out to  ____?</t>
-  </si>
-  <si>
     <t>Loop in  _____</t>
   </si>
   <si>
@@ -235,7 +232,28 @@
     <t xml:space="preserve">I'll give you back n minutes </t>
   </si>
   <si>
-    <t>[on a / It's been a] jouney</t>
+    <t>[on a / It's been a] journey</t>
+  </si>
+  <si>
+    <t>[We] can't see your screen</t>
+  </si>
+  <si>
+    <t>[Let's] take this offline</t>
+  </si>
+  <si>
+    <t>You're breaking up again</t>
+  </si>
+  <si>
+    <t>I'm having computer problems</t>
+  </si>
+  <si>
+    <t>Dog barking</t>
+  </si>
+  <si>
+    <t>on the same page</t>
+  </si>
+  <si>
+    <t>Can you reach out to  _____?</t>
   </si>
 </sst>
 </file>
@@ -811,10 +829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,12 +843,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -845,7 +863,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -855,7 +873,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -865,7 +883,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -875,17 +893,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -895,22 +913,22 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -920,7 +938,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -935,12 +953,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -950,87 +968,102 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1165,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1184,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1201,7 +1234,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1218,7 +1251,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1235,7 +1268,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -1268,7 +1301,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1320,7 +1353,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,7 +1370,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1354,7 +1387,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1371,7 +1404,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Removed a dup phrase from list and added a request for suggestions to the email message.
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="72">
   <si>
     <t>headers</t>
   </si>
@@ -154,9 +154,6 @@
     <t>low hanging fruit</t>
   </si>
   <si>
-    <t>I’ve got to jump on another call</t>
-  </si>
-  <si>
     <t>at the end of the day</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">I'll give you back n minutes </t>
-  </si>
-  <si>
-    <t>[on a / It's been a] journey</t>
   </si>
   <si>
     <t>[We] can't see your screen</t>
@@ -829,10 +823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,12 +837,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -863,7 +857,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -873,7 +867,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -893,17 +887,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -923,12 +917,12 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -938,7 +932,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -953,12 +947,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -968,32 +962,32 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -1003,12 +997,12 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1018,52 +1012,42 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1149,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1217,7 +1201,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1234,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1251,7 +1235,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1301,7 +1285,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1353,7 +1337,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,7 +1354,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1387,7 +1371,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Added a cliche and tweaked others
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u037679\Documents\AnacondaProjects\conference-call-bingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\conference-call-bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
   <si>
     <t>headers</t>
   </si>
@@ -175,9 +175,6 @@
     <t xml:space="preserve">I'll give you back x minutes </t>
   </si>
   <si>
-    <t>Can you repeat? I was multi-tasking</t>
-  </si>
-  <si>
     <t>Keep _____ in the loop</t>
   </si>
   <si>
@@ -247,10 +244,22 @@
     <t>on the same page</t>
   </si>
   <si>
-    <t>Can you reach out to  _____?</t>
-  </si>
-  <si>
     <t>I'm having technical difficulties</t>
+  </si>
+  <si>
+    <t>Can you / everyone see my screen?</t>
+  </si>
+  <si>
+    <t>I was multi-tasking</t>
+  </si>
+  <si>
+    <t>Echo / feedback / cutting out</t>
+  </si>
+  <si>
+    <t>Wind / road noise</t>
+  </si>
+  <si>
+    <t>Reach out to  _____</t>
   </si>
 </sst>
 </file>
@@ -723,7 +732,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Tuesday</v>
+        <v>Happy Thursday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -828,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +869,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -870,7 +879,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -885,22 +894,22 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -920,22 +929,22 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -945,7 +954,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -955,7 +964,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -965,22 +974,22 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -990,7 +999,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -1005,7 +1014,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1015,47 +1024,47 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1157,7 +1166,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1226,7 +1235,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1293,7 +1302,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1362,7 +1371,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added a 11 phrases and tweaked 3.
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u037679\Documents\AnacondaProjects\conference-call-bingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\conference-call-bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
   <si>
     <t>headers</t>
   </si>
@@ -181,9 +181,6 @@
     <t>awkward silence</t>
   </si>
   <si>
-    <t>I’ll take silence as a “no”</t>
-  </si>
-  <si>
     <t>col0</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>[Let's] take this offline</t>
   </si>
   <si>
-    <t>You're breaking up again</t>
-  </si>
-  <si>
     <t>I'm having computer problems</t>
   </si>
   <si>
@@ -262,7 +256,49 @@
     <t>Reach out to  _____</t>
   </si>
   <si>
-    <t>have / had to drop</t>
+    <t>My outlook / WebEx is not working</t>
+  </si>
+  <si>
+    <t>Unnecessary verbing ("Let's solution that")</t>
+  </si>
+  <si>
+    <t>I’ll take silence as _____</t>
+  </si>
+  <si>
+    <t>You're breaking up</t>
+  </si>
+  <si>
+    <t>It's on my radar</t>
+  </si>
+  <si>
+    <t>It is what it is</t>
+  </si>
+  <si>
+    <t>Ping me</t>
+  </si>
+  <si>
+    <t>[I don't] have the bandwidth</t>
+  </si>
+  <si>
+    <t>Ducks in a row</t>
+  </si>
+  <si>
+    <t>Chewing sounds</t>
+  </si>
+  <si>
+    <t>Animal or child sounds</t>
+  </si>
+  <si>
+    <t>You cut out</t>
+  </si>
+  <si>
+    <t>It's loading</t>
+  </si>
+  <si>
+    <t>Next slide please</t>
+  </si>
+  <si>
+    <t>I have / they had to drop</t>
   </si>
 </sst>
 </file>
@@ -699,7 +735,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +898,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -872,7 +908,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -882,7 +918,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -897,22 +933,22 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -932,22 +968,22 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -957,7 +993,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -967,7 +1003,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -977,22 +1013,22 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -1002,7 +1038,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -1017,7 +1053,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1037,42 +1073,97 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1174,7 +1265,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1243,7 +1334,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1310,7 +1401,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1379,7 +1470,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Small changes to existing phrases
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>headers</t>
   </si>
@@ -277,15 +277,6 @@
     <t>[I don't] have the bandwidth</t>
   </si>
   <si>
-    <t>Ducks in a row</t>
-  </si>
-  <si>
-    <t>Chewing sounds</t>
-  </si>
-  <si>
-    <t>Animal or child sounds</t>
-  </si>
-  <si>
     <t>You cut out</t>
   </si>
   <si>
@@ -299,6 +290,18 @@
   </si>
   <si>
     <t>…ping me / you</t>
+  </si>
+  <si>
+    <t>ducks in a row</t>
+  </si>
+  <si>
+    <t>chewing sounds</t>
+  </si>
+  <si>
+    <t>animal sounds</t>
+  </si>
+  <si>
+    <t>child sounds</t>
   </si>
 </sst>
 </file>
@@ -771,7 +774,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Wednesday</v>
+        <v>Happy Friday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -874,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -1128,7 +1131,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -1138,32 +1141,37 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Combined two similar phrases into one.
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -247,9 +247,6 @@
     <t>I was multi-tasking</t>
   </si>
   <si>
-    <t>Echo / feedback / cutting out</t>
-  </si>
-  <si>
     <t>Wind / road noise</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>[I don't] have the bandwidth</t>
   </si>
   <si>
-    <t>You cut out</t>
-  </si>
-  <si>
     <t>It's loading</t>
   </si>
   <si>
@@ -302,6 +296,12 @@
   </si>
   <si>
     <t>child sounds</t>
+  </si>
+  <si>
+    <t>echo / feedback</t>
+  </si>
+  <si>
+    <t>You're cutting out</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Friday</v>
+        <v>Happy Monday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -880,7 +880,7 @@
   <dimension ref="A1:A57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -1086,12 +1086,12 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -1111,67 +1111,67 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tweaks and de-dups
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
   <si>
     <t>headers</t>
   </si>
@@ -232,9 +232,6 @@
     <t>I'm having computer problems</t>
   </si>
   <si>
-    <t>Dog barking</t>
-  </si>
-  <si>
     <t>on the same page</t>
   </si>
   <si>
@@ -247,27 +244,18 @@
     <t>I was multi-tasking</t>
   </si>
   <si>
-    <t>Wind / road noise</t>
-  </si>
-  <si>
     <t>Reach out to  _____</t>
   </si>
   <si>
     <t>My outlook / WebEx is not working</t>
   </si>
   <si>
-    <t>Unnecessary verbing ("Let's solution that")</t>
-  </si>
-  <si>
     <t>I’ll take silence as _____</t>
   </si>
   <si>
     <t>You're breaking up</t>
   </si>
   <si>
-    <t>It's on my radar</t>
-  </si>
-  <si>
     <t>It is what it is</t>
   </si>
   <si>
@@ -302,6 +290,18 @@
   </si>
   <si>
     <t>You're cutting out</t>
+  </si>
+  <si>
+    <t>on the radar</t>
+  </si>
+  <si>
+    <t>wind / road noise</t>
+  </si>
+  <si>
+    <t>typing noise</t>
+  </si>
+  <si>
+    <t>unnecessary verbing ("Let's solution that")</t>
   </si>
 </sst>
 </file>
@@ -877,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -946,157 +946,157 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -1106,72 +1106,67 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added one and tweaked some others
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="92">
   <si>
     <t>headers</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Ok. Let's get started</t>
   </si>
   <si>
-    <t>Loop in  _____</t>
-  </si>
-  <si>
     <t>Is _____ on the call?</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t xml:space="preserve">I'll give you back x minutes </t>
   </si>
   <si>
-    <t>Keep _____ in the loop</t>
-  </si>
-  <si>
     <t>awkward silence</t>
   </si>
   <si>
@@ -244,33 +238,21 @@
     <t>I was multi-tasking</t>
   </si>
   <si>
-    <t>Reach out to  _____</t>
-  </si>
-  <si>
     <t>My outlook / WebEx is not working</t>
   </si>
   <si>
-    <t>I’ll take silence as _____</t>
-  </si>
-  <si>
     <t>You're breaking up</t>
   </si>
   <si>
     <t>It is what it is</t>
   </si>
   <si>
-    <t>[I don't] have the bandwidth</t>
-  </si>
-  <si>
     <t>It's loading</t>
   </si>
   <si>
     <t>Next slide please</t>
   </si>
   <si>
-    <t>I have / they had to drop</t>
-  </si>
-  <si>
     <t>…ping me / you</t>
   </si>
   <si>
@@ -292,9 +274,6 @@
     <t>You're cutting out</t>
   </si>
   <si>
-    <t>on the radar</t>
-  </si>
-  <si>
     <t>wind / road noise</t>
   </si>
   <si>
@@ -302,6 +281,33 @@
   </si>
   <si>
     <t>unnecessary verbing ("Let's solution that")</t>
+  </si>
+  <si>
+    <t>"voluntold"</t>
+  </si>
+  <si>
+    <t>on/off the radar</t>
+  </si>
+  <si>
+    <t>Loop in  ____</t>
+  </si>
+  <si>
+    <t>Keep ____ in the loop</t>
+  </si>
+  <si>
+    <t>I’ll take silence as ____</t>
+  </si>
+  <si>
+    <t>Reach out to  ____</t>
+  </si>
+  <si>
+    <t>Is ____ on the call?</t>
+  </si>
+  <si>
+    <t>I have to drop</t>
+  </si>
+  <si>
+    <t>have the bandwidth (i.e. work capacity)</t>
   </si>
 </sst>
 </file>
@@ -774,7 +780,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Monday</v>
+        <v>Happy Tuesday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -877,10 +883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,17 +897,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -911,17 +917,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -931,22 +937,22 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -956,32 +962,32 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -991,17 +997,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -1011,161 +1017,166 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1268,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1320,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1354,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1371,7 +1382,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -1404,7 +1415,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1456,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1473,7 +1484,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1490,7 +1501,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1507,7 +1518,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Added quotation marks where appropriate to distinguish from non-quotes
</commit_message>
<xml_diff>
--- a/BINGO_cc.xlsx
+++ b/BINGO_cc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="102">
   <si>
     <t>headers</t>
   </si>
@@ -142,33 +142,12 @@
     <t>Is _____ on the call?</t>
   </si>
   <si>
-    <t>Go ahead (talking at once)</t>
-  </si>
-  <si>
-    <t>It's [almost] Friday!</t>
-  </si>
-  <si>
-    <t>low hanging fruit</t>
-  </si>
-  <si>
-    <t>at the end of the day</t>
-  </si>
-  <si>
-    <t>Sorry I’m late (lame excuse)</t>
-  </si>
-  <si>
     <t>Can you email that to everyone</t>
   </si>
   <si>
     <t>Quotes</t>
   </si>
   <si>
-    <t>Happy [weekday]!</t>
-  </si>
-  <si>
-    <t>Let me IM them to see if they're joining</t>
-  </si>
-  <si>
     <t xml:space="preserve">I'll give you back x minutes </t>
   </si>
   <si>
@@ -181,84 +160,6 @@
     <t>Happy Wednesday</t>
   </si>
   <si>
-    <t>Can you email that to everyone?</t>
-  </si>
-  <si>
-    <t>Your phone was breaking up</t>
-  </si>
-  <si>
-    <t>Can you repeat the question?</t>
-  </si>
-  <si>
-    <t>Can everyone mute if you aren't talking?</t>
-  </si>
-  <si>
-    <t>I'll have to get back to you</t>
-  </si>
-  <si>
-    <t>(Starting) This won't take the whole time</t>
-  </si>
-  <si>
-    <t>win-win</t>
-  </si>
-  <si>
-    <t>circle back</t>
-  </si>
-  <si>
-    <t>touch base</t>
-  </si>
-  <si>
-    <t>level-set</t>
-  </si>
-  <si>
-    <t>I have a hard stop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I'll give you back n minutes </t>
-  </si>
-  <si>
-    <t>[We] can't see your screen</t>
-  </si>
-  <si>
-    <t>[Let's] take this offline</t>
-  </si>
-  <si>
-    <t>I'm having computer problems</t>
-  </si>
-  <si>
-    <t>on the same page</t>
-  </si>
-  <si>
-    <t>I'm having technical difficulties</t>
-  </si>
-  <si>
-    <t>Can you / everyone see my screen?</t>
-  </si>
-  <si>
-    <t>I was multi-tasking</t>
-  </si>
-  <si>
-    <t>My outlook / WebEx is not working</t>
-  </si>
-  <si>
-    <t>You're breaking up</t>
-  </si>
-  <si>
-    <t>It is what it is</t>
-  </si>
-  <si>
-    <t>It's loading</t>
-  </si>
-  <si>
-    <t>Next slide please</t>
-  </si>
-  <si>
-    <t>…ping me / you</t>
-  </si>
-  <si>
-    <t>ducks in a row</t>
-  </si>
-  <si>
     <t>chewing sounds</t>
   </si>
   <si>
@@ -271,9 +172,6 @@
     <t>echo / feedback</t>
   </si>
   <si>
-    <t>You're cutting out</t>
-  </si>
-  <si>
     <t>wind / road noise</t>
   </si>
   <si>
@@ -286,40 +184,160 @@
     <t>"voluntold"</t>
   </si>
   <si>
-    <t>on/off the radar</t>
-  </si>
-  <si>
-    <t>Loop in  ____</t>
-  </si>
-  <si>
-    <t>Keep ____ in the loop</t>
-  </si>
-  <si>
-    <t>I’ll take silence as ____</t>
-  </si>
-  <si>
-    <t>Reach out to  ____</t>
-  </si>
-  <si>
-    <t>Is ____ on the call?</t>
-  </si>
-  <si>
-    <t>I have to drop</t>
-  </si>
-  <si>
-    <t>have the bandwidth (i.e. work capacity)</t>
-  </si>
-  <si>
-    <t>(video) looking at wrong screen</t>
-  </si>
-  <si>
-    <t>(video) kid(s) walking around</t>
-  </si>
-  <si>
     <t>(video) animal(s) walking around</t>
   </si>
   <si>
     <t>(video) partner in view</t>
+  </si>
+  <si>
+    <t>"Happy [weekday]!"</t>
+  </si>
+  <si>
+    <t>"My outlook / WebEx is not working"</t>
+  </si>
+  <si>
+    <t>"I have to jump to another call"</t>
+  </si>
+  <si>
+    <t>"[We] can't see your screen"</t>
+  </si>
+  <si>
+    <t>"Can you email that to everyone?"</t>
+  </si>
+  <si>
+    <t>"Sorry I was on Mute"</t>
+  </si>
+  <si>
+    <t>"It's [almost] Friday!"</t>
+  </si>
+  <si>
+    <t>"[Let's] take this offline"</t>
+  </si>
+  <si>
+    <t>"I have a hard stop"</t>
+  </si>
+  <si>
+    <t>"Who just joined?"</t>
+  </si>
+  <si>
+    <t>"Go ahead" (talking at once)</t>
+  </si>
+  <si>
+    <t>"Is ____ on the call?"</t>
+  </si>
+  <si>
+    <t>"Your phone was breaking up"</t>
+  </si>
+  <si>
+    <t>"Can you repeat the question?"</t>
+  </si>
+  <si>
+    <t>"Please mute if you aren't talking"</t>
+  </si>
+  <si>
+    <t>"Can you hear me?"</t>
+  </si>
+  <si>
+    <t>"Can you / everyone see my screen?"</t>
+  </si>
+  <si>
+    <t>"Let me IM them to see if they're joining"</t>
+  </si>
+  <si>
+    <t>"You're not (are you) sharing(?)"</t>
+  </si>
+  <si>
+    <t>"I'll have to get back to you"</t>
+  </si>
+  <si>
+    <t>"Ok. Let's get started"</t>
+  </si>
+  <si>
+    <t>"I'll give you back n minutes "</t>
+  </si>
+  <si>
+    <t>"Reach out to  ____"</t>
+  </si>
+  <si>
+    <t>(Starting) "This won't take the whole time"</t>
+  </si>
+  <si>
+    <t>"level-set"</t>
+  </si>
+  <si>
+    <t>"Sorry I’m late" (lame excuse)</t>
+  </si>
+  <si>
+    <t>"I was multi-tasking"</t>
+  </si>
+  <si>
+    <t>"low hanging fruit"</t>
+  </si>
+  <si>
+    <t>"at the end of the day"</t>
+  </si>
+  <si>
+    <t>"win-win"</t>
+  </si>
+  <si>
+    <t>"Loop in  ____"</t>
+  </si>
+  <si>
+    <t>"Keep ____ in the loop"</t>
+  </si>
+  <si>
+    <t>"circle back"</t>
+  </si>
+  <si>
+    <t>"touch base"</t>
+  </si>
+  <si>
+    <t>"I’ll take silence as ____"</t>
+  </si>
+  <si>
+    <t>"You're breaking up"</t>
+  </si>
+  <si>
+    <t>"I'm having computer problems"</t>
+  </si>
+  <si>
+    <t>"on the same page"</t>
+  </si>
+  <si>
+    <t>"I'm having technical difficulties"</t>
+  </si>
+  <si>
+    <t>"I have to drop"</t>
+  </si>
+  <si>
+    <t>"on/off the radar"</t>
+  </si>
+  <si>
+    <t>"It is what it is"</t>
+  </si>
+  <si>
+    <t>"ping me / you"</t>
+  </si>
+  <si>
+    <t>"have the bandwidth" (i.e. work capacity)</t>
+  </si>
+  <si>
+    <t>"ducks in a row"</t>
+  </si>
+  <si>
+    <t>"You're cutting out"</t>
+  </si>
+  <si>
+    <t>"It's loading"</t>
+  </si>
+  <si>
+    <t>"Next slide please"</t>
+  </si>
+  <si>
+    <t>(video) never looking at camera</t>
+  </si>
+  <si>
+    <t>(video) kid(s) in view/interrupting</t>
   </si>
 </sst>
 </file>
@@ -792,7 +810,7 @@
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">"Happy "&amp;TEXT(TODAY(),"dddd")</f>
-        <v>Happy Tuesday</v>
+        <v>Happy Thursday</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -895,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,217 +927,217 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -1129,87 +1147,92 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1363,7 +1386,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,7 +1403,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1397,7 +1420,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1447,7 +1470,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1499,7 +1522,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1516,7 +1539,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1533,7 +1556,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>

</xml_diff>